<commit_message>
pre excel sheet update
</commit_message>
<xml_diff>
--- a/postuploads/postimages.xlsx
+++ b/postuploads/postimages.xlsx
@@ -7,9 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sector3" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sector1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,17 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="16"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,11 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -131,69 +122,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2381250" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2381250" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,68 +420,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="300" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>AzimuthCellSec3</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="300" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>AzimuthCellSec1</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>